<commit_message>
added Personalised workout plan
Personalised workout plan
</commit_message>
<xml_diff>
--- a/Learning/Python/Prompts_MasterSheet_MLGeeks.xlsx
+++ b/Learning/Python/Prompts_MasterSheet_MLGeeks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://infinera-my.sharepoint.com/personal/maagarwal_infinera_com/Documents/GenAI/2024_100Days/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maagarwal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{6788F120-C814-49A6-97DB-08F4FCC179D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7838ED0F-A3CA-408A-A590-05D5B4F7CDF5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB829B46-5358-4FA7-97D0-15B815DE7674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9454125C-940D-4C08-90D2-781987D4CC03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9454125C-940D-4C08-90D2-781987D4CC03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Use Case</t>
   </si>
@@ -102,6 +102,23 @@
   <si>
     <t>&lt;expertise level&gt;: begineer, intermediate
 &lt;specify the topic&gt;: Variables, list</t>
+  </si>
+  <si>
+    <t>You are a fitness expert with more than 15 years of experience.I need a personalized workout plan. I’m currently at an [insert fitness level] with [any current workout routine] and have [any recent injuries or health concerns]. My current weight is [current weight], and my target weight is [expected weight]. My primary goals are [insert fitness goals], targeting [specific target areas]. I prefer [preferred workout types] and enjoy activities like [enjoyable activities]. I can work out [available days per week] for [available time per session], and I have access to [equipment]. Please consider my [any dietary preferences or restrictions] and any other relevant information.</t>
+  </si>
+  <si>
+    <t>Personalised workout plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [insert fitness level]:
+[any current workout routine]:
+ [current weight]:
+ [insert fitness goals]:
+ [specific target areas]:
+ [available days per week]:
+ [available time per session]:
+ [equipment]:
+ [any dietary preferences or restrictions] :</t>
   </si>
 </sst>
 </file>
@@ -509,17 +526,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80B48C6-323C-41F1-8C93-EC7136C62D20}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="89.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -533,7 +550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="354" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -542,6 +559,17 @@
       </c>
       <c r="C2" s="4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>